<commit_message>
Party generators and inventory changer
</commit_message>
<xml_diff>
--- a/HUNT/Weapons/Weapons.xlsx
+++ b/HUNT/Weapons/Weapons.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>Auto-5</t>
   </si>
@@ -70,6 +70,45 @@
   </si>
   <si>
     <t>Close</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Высокая</t>
+  </si>
+  <si>
+    <t>Средняя</t>
+  </si>
+  <si>
+    <t>Низкая</t>
+  </si>
+  <si>
+    <t>С 18 по 12</t>
+  </si>
+  <si>
+    <t>С 33 по 20</t>
+  </si>
+  <si>
+    <t>С 11 по 7</t>
+  </si>
+  <si>
+    <t>С 6</t>
+  </si>
+  <si>
+    <t>С 27 по 17</t>
+  </si>
+  <si>
+    <t>С 16 по 10</t>
+  </si>
+  <si>
+    <t>С 9</t>
+  </si>
+  <si>
+    <t>С 14</t>
+  </si>
+  <si>
+    <t>С 19 по 15</t>
   </si>
 </sst>
 </file>
@@ -105,8 +144,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -408,18 +448,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E16"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" customWidth="1"/>
+    <col min="10" max="10" width="11" customWidth="1"/>
+    <col min="11" max="11" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
       <c r="C1" t="s">
         <v>15</v>
       </c>
@@ -429,8 +475,20 @@
       <c r="E1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -443,80 +501,134 @@
       <c r="E2">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
         <v>2</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>4</v>
-      </c>
-      <c r="E6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
       <c r="E7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C8">
         <v>4</v>
@@ -525,30 +637,36 @@
         <v>3</v>
       </c>
       <c r="E8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D9">
         <v>3</v>
       </c>
       <c r="E9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
       <c r="D10">
         <v>3</v>
       </c>
@@ -556,88 +674,106 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C13">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D13">
         <v>2</v>
       </c>
       <c r="E13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
         <v>4</v>
       </c>
-      <c r="D14">
-        <v>3</v>
-      </c>
       <c r="E14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C15">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D15">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="E16">
         <v>2</v>
       </c>
-      <c r="D16">
-        <v>3</v>
-      </c>
-      <c r="E16">
-        <v>3</v>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>